<commit_message>
Se actualiza el feature de registro para agregar los escenarios sad path
</commit_message>
<xml_diff>
--- a/Test Plan App Contenido.xlsx
+++ b/Test Plan App Contenido.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ERIK\AUTOMATIZACION-JAVA\GIT_HUB\MOBILE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ERIK\AUTOMATIZACION-JAVA\GIT_HUB\MOBILE\qa-mobile-app-content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8E4EC3-EF29-4B5C-8F00-B07115FBAB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E5C83A-EF36-448C-94B1-313C26696E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="115">
   <si>
     <t>CALIDAD EN USO</t>
   </si>
@@ -699,9 +699,6 @@
     <t>Evidencia</t>
   </si>
   <si>
-    <t>observacion</t>
-  </si>
-  <si>
     <t>Exitoso</t>
   </si>
   <si>
@@ -853,6 +850,36 @@
   </si>
   <si>
     <t>Verificar que el texto SUBMIT aparezca centrado en el boton (VALIDACIONES LOOK AND FEEL)</t>
+  </si>
+  <si>
+    <t>Verificar que al diligenciar el formulario de registro con los datos correctos y le de clik al boton Submit, este presenta otra pantalla donde el registro es exitoso</t>
+  </si>
+  <si>
+    <t>Observacion</t>
+  </si>
+  <si>
+    <t>No presente mensaje de obligatoriedad</t>
+  </si>
+  <si>
+    <t>Esta validcion no la este presentando</t>
+  </si>
+  <si>
+    <t>No presente mensaje de diligenciar el campo</t>
+  </si>
+  <si>
+    <t>Esta permitiendo caracteres especiales</t>
+  </si>
+  <si>
+    <t>Solo permite un solo carácter especial</t>
+  </si>
+  <si>
+    <t>No se esta validando el mismo password al salir del foco del campo</t>
+  </si>
+  <si>
+    <t>No cumplen este regla</t>
+  </si>
+  <si>
+    <t>Verificar que al diligenciar el formulario de registro con los datos correctos del password y repeat passwo, sin diligenciar el username y le de clik al boton Submit, este NO debe presenta la pantalla donde el registro es exitoso</t>
   </si>
 </sst>
 </file>
@@ -1226,6 +1253,33 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1258,42 +1312,55 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF6D01"/>
+          <bgColor rgb="FFFF6D01"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBBC04"/>
+          <bgColor rgb="FFFBBC04"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF34A853"/>
+          <bgColor rgb="FF34A853"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA4335"/>
+          <bgColor rgb="FFEA4335"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1641,25 +1708,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1970,11 +2037,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1988,7 +2055,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="38" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1997,21 +2064,21 @@
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -3042,12 +3109,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -3064,7 +3131,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="44" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -3075,7 +3142,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
@@ -3084,14 +3151,14 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
@@ -3100,7 +3167,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="41" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -3109,28 +3176,28 @@
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="41" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -3139,21 +3206,21 @@
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="41" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -3161,13 +3228,13 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="41" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -3175,25 +3242,25 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="42" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -3201,7 +3268,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="6" t="s">
         <v>41</v>
       </c>
@@ -4204,15 +4271,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.08984375" customWidth="1"/>
-    <col min="2" max="2" width="76.08984375" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" customWidth="1"/>
+    <col min="2" max="2" width="75.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.08984375" customWidth="1"/>
     <col min="5" max="5" width="9.453125" customWidth="1"/>
     <col min="6" max="6" width="14.08984375" customWidth="1"/>
@@ -4220,26 +4287,26 @@
     <col min="8" max="8" width="14.90625" customWidth="1"/>
     <col min="9" max="9" width="14.08984375" customWidth="1"/>
     <col min="10" max="10" width="27.26953125" customWidth="1"/>
-    <col min="11" max="11" width="9.08984375" customWidth="1"/>
+    <col min="11" max="11" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.26953125" customWidth="1"/>
     <col min="19" max="19" width="16.453125" customWidth="1"/>
     <col min="20" max="20" width="6.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
       <c r="L1" s="8"/>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
@@ -4295,10 +4362,10 @@
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="39"/>
+      <c r="F4" s="48"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
@@ -4311,11 +4378,11 @@
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
-      <c r="E5" s="40">
+      <c r="E5" s="49">
         <f>((M17+O17+Q17+R17)-N17)/S17</f>
-        <v>6.9767441860465115E-2</v>
-      </c>
-      <c r="F5" s="39"/>
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="48"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
@@ -4546,72 +4613,72 @@
         <v>53</v>
       </c>
       <c r="K16" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="M16" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="M16" s="48" t="s">
+      <c r="N16" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="N16" s="49" t="s">
+      <c r="O16" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="O16" s="49" t="s">
+      <c r="P16" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="P16" s="49" t="s">
+      <c r="Q16" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="Q16" s="49" t="s">
+      <c r="R16" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="R16" s="49" t="s">
+      <c r="S16" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="S16" s="49" t="s">
+      <c r="T16" s="15"/>
+    </row>
+    <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="T16" s="15"/>
-    </row>
-    <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="39"/>
-      <c r="M17" s="50">
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="48"/>
+      <c r="M17" s="34">
         <f>+COUNTIF(F:F,M16)</f>
-        <v>1</v>
-      </c>
-      <c r="N17" s="50">
+        <v>36</v>
+      </c>
+      <c r="N17" s="34">
         <f>+COUNTIF(F:F,N16)</f>
-        <v>1</v>
-      </c>
-      <c r="O17" s="50">
+        <v>9</v>
+      </c>
+      <c r="O17" s="34">
         <f>+COUNTIF(F:F,O16)</f>
-        <v>1</v>
-      </c>
-      <c r="P17" s="50">
+        <v>0</v>
+      </c>
+      <c r="P17" s="34">
         <f>+COUNTIF(F:F,P16)</f>
-        <v>38</v>
-      </c>
-      <c r="Q17" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="34">
         <f>+COUNTIF(F:F,Q16)</f>
-        <v>1</v>
-      </c>
-      <c r="R17" s="50">
+        <v>0</v>
+      </c>
+      <c r="R17" s="34">
         <f>+COUNTIF(F:F,R16)</f>
-        <v>1</v>
-      </c>
-      <c r="S17" s="50">
+        <v>0</v>
+      </c>
+      <c r="S17" s="34">
         <f t="shared" ref="S17:S18" si="0">SUM(M17:R17)</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="T17" s="18"/>
     </row>
@@ -4619,45 +4686,45 @@
       <c r="A18" s="25">
         <v>1</v>
       </c>
-      <c r="B18" s="43" t="s">
-        <v>64</v>
+      <c r="B18" s="28" t="s">
+        <v>63</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="19"/>
       <c r="E18" s="21"/>
       <c r="F18" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="23"/>
       <c r="I18" s="23"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
-      <c r="M18" s="51">
+      <c r="M18" s="35">
         <f>+M17/S17</f>
-        <v>2.3255813953488372E-2</v>
-      </c>
-      <c r="N18" s="51">
+        <v>0.8</v>
+      </c>
+      <c r="N18" s="35">
         <f>+N17/S17</f>
-        <v>2.3255813953488372E-2</v>
-      </c>
-      <c r="O18" s="51">
+        <v>0.2</v>
+      </c>
+      <c r="O18" s="35">
         <f>+O17/S17</f>
-        <v>2.3255813953488372E-2</v>
-      </c>
-      <c r="P18" s="51">
+        <v>0</v>
+      </c>
+      <c r="P18" s="35">
         <f>+P17/S17</f>
-        <v>0.88372093023255816</v>
-      </c>
-      <c r="Q18" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="35">
         <f>+Q17/S17</f>
-        <v>2.3255813953488372E-2</v>
-      </c>
-      <c r="R18" s="51">
+        <v>0</v>
+      </c>
+      <c r="R18" s="35">
         <f>+R17/S17</f>
-        <v>2.3255813953488372E-2</v>
-      </c>
-      <c r="S18" s="51">
+        <v>0</v>
+      </c>
+      <c r="S18" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4668,40 +4735,40 @@
         <v>2</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="19"/>
       <c r="E19" s="21"/>
       <c r="F19" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="23"/>
       <c r="I19" s="23"/>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="42"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
+      <c r="T19" s="27"/>
     </row>
     <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
         <v>3</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="19"/>
       <c r="E20" s="21"/>
       <c r="F20" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="23"/>
@@ -4715,20 +4782,20 @@
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
       <c r="S20" s="24"/>
-      <c r="T20" s="42"/>
+      <c r="T20" s="27"/>
     </row>
     <row r="21" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
         <v>4</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="19"/>
       <c r="E21" s="21"/>
       <c r="F21" s="20" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="23"/>
@@ -4742,20 +4809,20 @@
       <c r="Q21" s="24"/>
       <c r="R21" s="24"/>
       <c r="S21" s="24"/>
-      <c r="T21" s="42"/>
+      <c r="T21" s="27"/>
     </row>
     <row r="22" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <v>5</v>
       </c>
-      <c r="B22" s="46" t="s">
-        <v>91</v>
+      <c r="B22" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="19"/>
       <c r="E22" s="21"/>
       <c r="F22" s="20" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="23"/>
@@ -4769,26 +4836,28 @@
       <c r="Q22" s="24"/>
       <c r="R22" s="24"/>
       <c r="S22" s="24"/>
-      <c r="T22" s="42"/>
+      <c r="T22" s="27"/>
     </row>
     <row r="23" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25">
         <v>6</v>
       </c>
-      <c r="B23" s="45" t="s">
-        <v>76</v>
+      <c r="B23" s="29" t="s">
+        <v>75</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="19"/>
       <c r="E23" s="21"/>
       <c r="F23" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
       <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
+      <c r="K23" s="19" t="s">
+        <v>107</v>
+      </c>
       <c r="M23" s="24"/>
       <c r="N23" s="24"/>
       <c r="O23" s="24"/>
@@ -4796,20 +4865,20 @@
       <c r="Q23" s="24"/>
       <c r="R23" s="24"/>
       <c r="S23" s="24"/>
-      <c r="T23" s="42"/>
+      <c r="T23" s="27"/>
     </row>
     <row r="24" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
         <v>7</v>
       </c>
-      <c r="B24" s="45" t="s">
-        <v>77</v>
+      <c r="B24" s="29" t="s">
+        <v>76</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="19"/>
       <c r="E24" s="21"/>
       <c r="F24" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="23"/>
@@ -4823,20 +4892,20 @@
       <c r="Q24" s="24"/>
       <c r="R24" s="24"/>
       <c r="S24" s="24"/>
-      <c r="T24" s="42"/>
+      <c r="T24" s="27"/>
     </row>
     <row r="25" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25">
         <v>8</v>
       </c>
-      <c r="B25" s="45" t="s">
-        <v>75</v>
+      <c r="B25" s="29" t="s">
+        <v>74</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="19"/>
       <c r="E25" s="21"/>
       <c r="F25" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="23"/>
@@ -4850,20 +4919,20 @@
       <c r="Q25" s="24"/>
       <c r="R25" s="24"/>
       <c r="S25" s="24"/>
-      <c r="T25" s="42"/>
+      <c r="T25" s="27"/>
     </row>
     <row r="26" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>9</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" s="20"/>
       <c r="D26" s="19"/>
       <c r="E26" s="21"/>
       <c r="F26" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="23"/>
@@ -4877,20 +4946,20 @@
       <c r="Q26" s="24"/>
       <c r="R26" s="24"/>
       <c r="S26" s="24"/>
-      <c r="T26" s="42"/>
+      <c r="T26" s="27"/>
     </row>
     <row r="27" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25">
         <v>10</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="20"/>
       <c r="D27" s="19"/>
       <c r="E27" s="21"/>
       <c r="F27" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="23"/>
@@ -4904,26 +4973,28 @@
       <c r="Q27" s="24"/>
       <c r="R27" s="24"/>
       <c r="S27" s="24"/>
-      <c r="T27" s="42"/>
+      <c r="T27" s="27"/>
     </row>
     <row r="28" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25">
         <v>11</v>
       </c>
-      <c r="B28" s="47" t="s">
-        <v>88</v>
+      <c r="B28" s="31" t="s">
+        <v>87</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="19"/>
       <c r="E28" s="21"/>
       <c r="F28" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="23"/>
       <c r="I28" s="23"/>
       <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
+      <c r="K28" s="19" t="s">
+        <v>108</v>
+      </c>
       <c r="M28" s="24"/>
       <c r="N28" s="24"/>
       <c r="O28" s="24"/>
@@ -4931,26 +5002,28 @@
       <c r="Q28" s="24"/>
       <c r="R28" s="24"/>
       <c r="S28" s="24"/>
-      <c r="T28" s="42"/>
+      <c r="T28" s="27"/>
     </row>
     <row r="29" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25">
         <v>12</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="19"/>
       <c r="E29" s="21"/>
       <c r="F29" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="23"/>
       <c r="I29" s="23"/>
       <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
+      <c r="K29" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="M29" s="24"/>
       <c r="N29" s="24"/>
       <c r="O29" s="24"/>
@@ -4958,20 +5031,20 @@
       <c r="Q29" s="24"/>
       <c r="R29" s="24"/>
       <c r="S29" s="24"/>
-      <c r="T29" s="42"/>
+      <c r="T29" s="27"/>
     </row>
     <row r="30" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25">
         <v>13</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="19"/>
       <c r="E30" s="21"/>
       <c r="F30" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="23"/>
@@ -4985,26 +5058,28 @@
       <c r="Q30" s="24"/>
       <c r="R30" s="24"/>
       <c r="S30" s="24"/>
-      <c r="T30" s="42"/>
+      <c r="T30" s="27"/>
     </row>
     <row r="31" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25">
         <v>14</v>
       </c>
-      <c r="B31" s="46" t="s">
-        <v>92</v>
+      <c r="B31" s="30" t="s">
+        <v>91</v>
       </c>
       <c r="C31" s="20"/>
       <c r="D31" s="19"/>
       <c r="E31" s="21"/>
       <c r="F31" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="23"/>
       <c r="I31" s="23"/>
       <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
+      <c r="K31" s="19" t="s">
+        <v>110</v>
+      </c>
       <c r="M31" s="24"/>
       <c r="N31" s="24"/>
       <c r="O31" s="24"/>
@@ -5012,20 +5087,20 @@
       <c r="Q31" s="24"/>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
-      <c r="T31" s="42"/>
+      <c r="T31" s="27"/>
     </row>
     <row r="32" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25">
         <v>15</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32" s="20"/>
       <c r="D32" s="19"/>
       <c r="E32" s="21"/>
       <c r="F32" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="23"/>
@@ -5039,20 +5114,20 @@
       <c r="Q32" s="24"/>
       <c r="R32" s="24"/>
       <c r="S32" s="24"/>
-      <c r="T32" s="42"/>
+      <c r="T32" s="27"/>
     </row>
     <row r="33" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25">
         <v>16</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" s="20"/>
       <c r="D33" s="19"/>
       <c r="E33" s="21"/>
       <c r="F33" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="23"/>
@@ -5066,20 +5141,20 @@
       <c r="Q33" s="24"/>
       <c r="R33" s="24"/>
       <c r="S33" s="24"/>
-      <c r="T33" s="42"/>
+      <c r="T33" s="27"/>
     </row>
     <row r="34" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25">
         <v>17</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" s="20"/>
       <c r="D34" s="19"/>
       <c r="E34" s="21"/>
       <c r="F34" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="23"/>
@@ -5093,20 +5168,20 @@
       <c r="Q34" s="24"/>
       <c r="R34" s="24"/>
       <c r="S34" s="24"/>
-      <c r="T34" s="42"/>
+      <c r="T34" s="27"/>
     </row>
     <row r="35" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25">
         <v>18</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35" s="20"/>
       <c r="D35" s="19"/>
       <c r="E35" s="21"/>
       <c r="F35" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="23"/>
@@ -5120,26 +5195,28 @@
       <c r="Q35" s="24"/>
       <c r="R35" s="24"/>
       <c r="S35" s="24"/>
-      <c r="T35" s="42"/>
+      <c r="T35" s="27"/>
     </row>
     <row r="36" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25">
         <v>19</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="20"/>
       <c r="D36" s="19"/>
       <c r="E36" s="21"/>
       <c r="F36" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
       <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
+      <c r="K36" s="19" t="s">
+        <v>111</v>
+      </c>
       <c r="M36" s="24"/>
       <c r="N36" s="24"/>
       <c r="O36" s="24"/>
@@ -5147,20 +5224,20 @@
       <c r="Q36" s="24"/>
       <c r="R36" s="24"/>
       <c r="S36" s="24"/>
-      <c r="T36" s="42"/>
+      <c r="T36" s="27"/>
     </row>
     <row r="37" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25">
         <v>20</v>
       </c>
-      <c r="B37" s="46" t="s">
-        <v>93</v>
+      <c r="B37" s="30" t="s">
+        <v>92</v>
       </c>
       <c r="C37" s="20"/>
       <c r="D37" s="19"/>
       <c r="E37" s="21"/>
       <c r="F37" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="23"/>
@@ -5174,20 +5251,20 @@
       <c r="Q37" s="24"/>
       <c r="R37" s="24"/>
       <c r="S37" s="24"/>
-      <c r="T37" s="42"/>
+      <c r="T37" s="27"/>
     </row>
     <row r="38" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="25">
         <v>21</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C38" s="20"/>
       <c r="D38" s="19"/>
       <c r="E38" s="21"/>
       <c r="F38" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="23"/>
@@ -5201,20 +5278,20 @@
       <c r="Q38" s="24"/>
       <c r="R38" s="24"/>
       <c r="S38" s="24"/>
-      <c r="T38" s="42"/>
+      <c r="T38" s="27"/>
     </row>
     <row r="39" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25">
         <v>22</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" s="20"/>
       <c r="D39" s="19"/>
       <c r="E39" s="21"/>
       <c r="F39" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="23"/>
@@ -5228,20 +5305,20 @@
       <c r="Q39" s="24"/>
       <c r="R39" s="24"/>
       <c r="S39" s="24"/>
-      <c r="T39" s="42"/>
+      <c r="T39" s="27"/>
     </row>
     <row r="40" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="25">
         <v>23</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" s="20"/>
       <c r="D40" s="19"/>
       <c r="E40" s="21"/>
       <c r="F40" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="23"/>
@@ -5255,20 +5332,20 @@
       <c r="Q40" s="24"/>
       <c r="R40" s="24"/>
       <c r="S40" s="24"/>
-      <c r="T40" s="42"/>
+      <c r="T40" s="27"/>
     </row>
     <row r="41" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25">
         <v>24</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" s="20"/>
       <c r="D41" s="19"/>
       <c r="E41" s="21"/>
       <c r="F41" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="23"/>
@@ -5282,20 +5359,20 @@
       <c r="Q41" s="24"/>
       <c r="R41" s="24"/>
       <c r="S41" s="24"/>
-      <c r="T41" s="42"/>
+      <c r="T41" s="27"/>
     </row>
     <row r="42" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="25">
         <v>25</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" s="20"/>
       <c r="D42" s="19"/>
       <c r="E42" s="21"/>
       <c r="F42" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G42" s="22"/>
       <c r="H42" s="23"/>
@@ -5309,26 +5386,28 @@
       <c r="Q42" s="24"/>
       <c r="R42" s="24"/>
       <c r="S42" s="24"/>
-      <c r="T42" s="42"/>
+      <c r="T42" s="27"/>
     </row>
     <row r="43" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25">
         <v>26</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C43" s="20"/>
       <c r="D43" s="19"/>
       <c r="E43" s="21"/>
       <c r="F43" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="23"/>
       <c r="I43" s="23"/>
       <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
+      <c r="K43" s="19" t="s">
+        <v>112</v>
+      </c>
       <c r="M43" s="24"/>
       <c r="N43" s="24"/>
       <c r="O43" s="24"/>
@@ -5336,20 +5415,20 @@
       <c r="Q43" s="24"/>
       <c r="R43" s="24"/>
       <c r="S43" s="24"/>
-      <c r="T43" s="42"/>
+      <c r="T43" s="27"/>
     </row>
     <row r="44" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25">
         <v>27</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C44" s="20"/>
       <c r="D44" s="19"/>
       <c r="E44" s="21"/>
       <c r="F44" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="23"/>
@@ -5363,20 +5442,20 @@
       <c r="Q44" s="24"/>
       <c r="R44" s="24"/>
       <c r="S44" s="24"/>
-      <c r="T44" s="42"/>
+      <c r="T44" s="27"/>
     </row>
     <row r="45" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25">
         <v>28</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C45" s="20"/>
       <c r="D45" s="19"/>
       <c r="E45" s="21"/>
       <c r="F45" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="23"/>
@@ -5390,20 +5469,20 @@
       <c r="Q45" s="24"/>
       <c r="R45" s="24"/>
       <c r="S45" s="24"/>
-      <c r="T45" s="42"/>
+      <c r="T45" s="27"/>
     </row>
     <row r="46" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="25">
         <v>29</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" s="20"/>
       <c r="D46" s="19"/>
       <c r="E46" s="21"/>
       <c r="F46" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="23"/>
@@ -5417,26 +5496,28 @@
       <c r="Q46" s="24"/>
       <c r="R46" s="24"/>
       <c r="S46" s="24"/>
-      <c r="T46" s="42"/>
+      <c r="T46" s="27"/>
     </row>
     <row r="47" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="25">
         <v>30</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C47" s="20"/>
       <c r="D47" s="19"/>
       <c r="E47" s="21"/>
       <c r="F47" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="23"/>
       <c r="I47" s="23"/>
       <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
+      <c r="K47" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="M47" s="24"/>
       <c r="N47" s="24"/>
       <c r="O47" s="24"/>
@@ -5444,20 +5525,20 @@
       <c r="Q47" s="24"/>
       <c r="R47" s="24"/>
       <c r="S47" s="24"/>
-      <c r="T47" s="42"/>
+      <c r="T47" s="27"/>
     </row>
     <row r="48" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="25">
         <v>31</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C48" s="20"/>
       <c r="D48" s="19"/>
       <c r="E48" s="21"/>
       <c r="F48" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="23"/>
@@ -5471,20 +5552,20 @@
       <c r="Q48" s="24"/>
       <c r="R48" s="24"/>
       <c r="S48" s="24"/>
-      <c r="T48" s="42"/>
+      <c r="T48" s="27"/>
     </row>
     <row r="49" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="25">
         <v>32</v>
       </c>
-      <c r="B49" s="46" t="s">
-        <v>94</v>
+      <c r="B49" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="C49" s="20"/>
       <c r="D49" s="19"/>
       <c r="E49" s="21"/>
       <c r="F49" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="23"/>
@@ -5498,20 +5579,20 @@
       <c r="Q49" s="24"/>
       <c r="R49" s="24"/>
       <c r="S49" s="24"/>
-      <c r="T49" s="42"/>
+      <c r="T49" s="27"/>
     </row>
     <row r="50" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="25">
         <v>33</v>
       </c>
-      <c r="B50" s="46" t="s">
-        <v>97</v>
+      <c r="B50" s="30" t="s">
+        <v>96</v>
       </c>
       <c r="C50" s="20"/>
       <c r="D50" s="19"/>
       <c r="E50" s="21"/>
       <c r="F50" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="23"/>
@@ -5525,20 +5606,20 @@
       <c r="Q50" s="24"/>
       <c r="R50" s="24"/>
       <c r="S50" s="24"/>
-      <c r="T50" s="42"/>
+      <c r="T50" s="27"/>
     </row>
     <row r="51" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="25">
         <v>34</v>
       </c>
-      <c r="B51" s="46" t="s">
-        <v>95</v>
+      <c r="B51" s="30" t="s">
+        <v>94</v>
       </c>
       <c r="C51" s="20"/>
       <c r="D51" s="19"/>
       <c r="E51" s="21"/>
       <c r="F51" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="23"/>
@@ -5552,20 +5633,20 @@
       <c r="Q51" s="24"/>
       <c r="R51" s="24"/>
       <c r="S51" s="24"/>
-      <c r="T51" s="42"/>
+      <c r="T51" s="27"/>
     </row>
     <row r="52" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="25">
         <v>35</v>
       </c>
-      <c r="B52" s="46" t="s">
-        <v>96</v>
+      <c r="B52" s="30" t="s">
+        <v>95</v>
       </c>
       <c r="C52" s="20"/>
       <c r="D52" s="19"/>
       <c r="E52" s="21"/>
       <c r="F52" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="23"/>
@@ -5579,20 +5660,20 @@
       <c r="Q52" s="24"/>
       <c r="R52" s="24"/>
       <c r="S52" s="24"/>
-      <c r="T52" s="42"/>
+      <c r="T52" s="27"/>
     </row>
     <row r="53" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="25">
         <v>36</v>
       </c>
-      <c r="B53" s="46" t="s">
-        <v>98</v>
+      <c r="B53" s="30" t="s">
+        <v>97</v>
       </c>
       <c r="C53" s="20"/>
       <c r="D53" s="19"/>
       <c r="E53" s="21"/>
       <c r="F53" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="23"/>
@@ -5606,20 +5687,20 @@
       <c r="Q53" s="24"/>
       <c r="R53" s="24"/>
       <c r="S53" s="24"/>
-      <c r="T53" s="42"/>
+      <c r="T53" s="27"/>
     </row>
     <row r="54" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="25">
         <v>37</v>
       </c>
-      <c r="B54" s="46" t="s">
-        <v>99</v>
+      <c r="B54" s="30" t="s">
+        <v>98</v>
       </c>
       <c r="C54" s="20"/>
       <c r="D54" s="19"/>
       <c r="E54" s="21"/>
       <c r="F54" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="23"/>
@@ -5633,20 +5714,20 @@
       <c r="Q54" s="24"/>
       <c r="R54" s="24"/>
       <c r="S54" s="24"/>
-      <c r="T54" s="42"/>
+      <c r="T54" s="27"/>
     </row>
     <row r="55" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="25">
         <v>38</v>
       </c>
-      <c r="B55" s="46" t="s">
-        <v>100</v>
+      <c r="B55" s="30" t="s">
+        <v>99</v>
       </c>
       <c r="C55" s="20"/>
       <c r="D55" s="19"/>
       <c r="E55" s="21"/>
       <c r="F55" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="23"/>
@@ -5660,20 +5741,20 @@
       <c r="Q55" s="24"/>
       <c r="R55" s="24"/>
       <c r="S55" s="24"/>
-      <c r="T55" s="42"/>
+      <c r="T55" s="27"/>
     </row>
     <row r="56" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="25">
         <v>39</v>
       </c>
-      <c r="B56" s="46" t="s">
-        <v>101</v>
+      <c r="B56" s="30" t="s">
+        <v>100</v>
       </c>
       <c r="C56" s="20"/>
       <c r="D56" s="19"/>
       <c r="E56" s="21"/>
       <c r="F56" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="23"/>
@@ -5687,20 +5768,20 @@
       <c r="Q56" s="24"/>
       <c r="R56" s="24"/>
       <c r="S56" s="24"/>
-      <c r="T56" s="42"/>
+      <c r="T56" s="27"/>
     </row>
     <row r="57" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="25">
         <v>40</v>
       </c>
-      <c r="B57" s="46" t="s">
-        <v>102</v>
+      <c r="B57" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C57" s="20"/>
       <c r="D57" s="19"/>
       <c r="E57" s="21"/>
       <c r="F57" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="23"/>
@@ -5714,20 +5795,20 @@
       <c r="Q57" s="24"/>
       <c r="R57" s="24"/>
       <c r="S57" s="24"/>
-      <c r="T57" s="42"/>
+      <c r="T57" s="27"/>
     </row>
     <row r="58" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="25">
         <v>41</v>
       </c>
-      <c r="B58" s="46" t="s">
-        <v>103</v>
+      <c r="B58" s="30" t="s">
+        <v>102</v>
       </c>
       <c r="C58" s="20"/>
       <c r="D58" s="19"/>
       <c r="E58" s="21"/>
       <c r="F58" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="23"/>
@@ -5741,20 +5822,20 @@
       <c r="Q58" s="24"/>
       <c r="R58" s="24"/>
       <c r="S58" s="24"/>
-      <c r="T58" s="42"/>
+      <c r="T58" s="27"/>
     </row>
     <row r="59" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="25">
         <v>42</v>
       </c>
-      <c r="B59" s="46" t="s">
-        <v>104</v>
+      <c r="B59" s="30" t="s">
+        <v>103</v>
       </c>
       <c r="C59" s="20"/>
       <c r="D59" s="19"/>
       <c r="E59" s="21"/>
       <c r="F59" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="23"/>
@@ -5768,20 +5849,20 @@
       <c r="Q59" s="24"/>
       <c r="R59" s="24"/>
       <c r="S59" s="24"/>
-      <c r="T59" s="42"/>
+      <c r="T59" s="27"/>
     </row>
     <row r="60" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="25">
         <v>43</v>
       </c>
-      <c r="B60" s="46" t="s">
-        <v>105</v>
+      <c r="B60" s="30" t="s">
+        <v>104</v>
       </c>
       <c r="C60" s="20"/>
       <c r="D60" s="19"/>
       <c r="E60" s="21"/>
       <c r="F60" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="23"/>
@@ -5795,10 +5876,62 @@
       <c r="Q60" s="24"/>
       <c r="R60" s="24"/>
       <c r="S60" s="24"/>
-      <c r="T60" s="42"/>
-    </row>
-    <row r="61" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="T60" s="27"/>
+    </row>
+    <row r="61" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="25">
+        <v>44</v>
+      </c>
+      <c r="B61" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="20"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G61" s="22"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+      <c r="M61" s="24"/>
+      <c r="N61" s="24"/>
+      <c r="O61" s="24"/>
+      <c r="P61" s="24"/>
+      <c r="Q61" s="24"/>
+      <c r="R61" s="24"/>
+      <c r="S61" s="24"/>
+      <c r="T61" s="27"/>
+    </row>
+    <row r="62" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="25">
+        <v>45</v>
+      </c>
+      <c r="B62" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="20"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G62" s="22"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="23"/>
+      <c r="J62" s="19"/>
+      <c r="K62" s="19"/>
+      <c r="M62" s="24"/>
+      <c r="N62" s="24"/>
+      <c r="O62" s="24"/>
+      <c r="P62" s="24"/>
+      <c r="Q62" s="24"/>
+      <c r="R62" s="24"/>
+      <c r="S62" s="24"/>
+      <c r="T62" s="27"/>
+    </row>
     <row r="63" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6745,27 +6878,46 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="A17:K17"/>
   </mergeCells>
-  <conditionalFormatting sqref="F1:F1001">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Re-ejecutado">
+  <conditionalFormatting sqref="F1:F62">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Re-ejecutado">
       <formula>NOT(ISERROR(SEARCH(("Re-ejecutado"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F3 F12:F16 F18:F1001">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Fallido">
+  <conditionalFormatting sqref="F2:F3 F12:F16">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Fallido">
       <formula>NOT(ISERROR(SEARCH(("Fallido"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Exitoso">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Exitoso">
       <formula>NOT(ISERROR(SEARCH(("Exitoso"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="En proceso">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="En proceso">
       <formula>NOT(ISERROR(SEARCH(("En proceso"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH(("NA"),(F2))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F18:F1001">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Fallido">
+      <formula>NOT(ISERROR(SEARCH(("Fallido"),(F18))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Exitoso">
+      <formula>NOT(ISERROR(SEARCH(("Exitoso"),(F18))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="En proceso">
+      <formula>NOT(ISERROR(SEARCH(("En proceso"),(F18))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH(("NA"),(F18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F61:F1001">
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="Re-ejecutado">
+      <formula>NOT(ISERROR(SEARCH(("Re-ejecutado"),(F61))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="F18:F60" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="F18:F62" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"Exitoso,Fallido,En proceso,Sin iniciar,NA,Re-ejecutado"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>